<commit_message>
Move data properties for scripts to a separate partial class for readability
</commit_message>
<xml_diff>
--- a/doc/Research/ScenarioResearch2.xlsx
+++ b/doc/Research/ScenarioResearch2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronal\source\openh2\doc\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FA14BBF-53F5-480C-AFED-732758A2A4A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5203DE-F394-42D9-ABF0-6AC7BA7D7CE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{FB4B14C3-B7AC-492E-BB32-091DF86F0D58}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{FB4B14C3-B7AC-492E-BB32-091DF86F0D58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="132">
   <si>
     <t>Cao Location</t>
   </si>
@@ -201,9 +201,6 @@
     <t>same as above</t>
   </si>
   <si>
-    <t>strings with floats</t>
-  </si>
-  <si>
     <t>e3_coil_destroy</t>
   </si>
   <si>
@@ -403,6 +400,42 @@
   </si>
   <si>
     <t>no idea</t>
+  </si>
+  <si>
+    <t>Actual Scripts</t>
+  </si>
+  <si>
+    <t>Magic</t>
+  </si>
+  <si>
+    <t>Literal Pos</t>
+  </si>
+  <si>
+    <t>Magic Pos</t>
+  </si>
+  <si>
+    <t>Magic Scripts</t>
+  </si>
+  <si>
+    <t>strings with floats, LocationFlag</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Trigger</t>
+  </si>
+  <si>
+    <t>Emotion, StringIds?</t>
+  </si>
+  <si>
+    <t>72 is objects table?</t>
+  </si>
+  <si>
+    <t>obj72s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">376 is character tag references </t>
   </si>
 </sst>
 </file>
@@ -512,13 +545,17 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -866,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1D70A5-77EB-4101-A684-C29A663B6757}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,7 +1055,7 @@
         <v>120</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="2"/>
@@ -1030,7 +1067,7 @@
         <v>128</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="2"/>
@@ -1081,7 +1118,7 @@
         <v>72</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="1"/>
@@ -1236,7 +1273,7 @@
         <v>248</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="2"/>
@@ -1416,7 +1453,7 @@
         <v>336</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="2"/>
@@ -1428,7 +1465,7 @@
         <v>344</v>
       </c>
       <c r="F23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="2"/>
@@ -1440,7 +1477,7 @@
         <v>352</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="2"/>
@@ -1452,7 +1489,7 @@
         <v>360</v>
       </c>
       <c r="F25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="2"/>
@@ -1464,7 +1501,7 @@
         <v>368</v>
       </c>
       <c r="F26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="2"/>
@@ -1476,7 +1513,7 @@
         <v>376</v>
       </c>
       <c r="F27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="2"/>
@@ -1501,7 +1538,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G28" t="s">
         <v>21</v>
@@ -1520,7 +1557,7 @@
         <v>456</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="2"/>
@@ -1542,7 +1579,7 @@
         <v>128</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="1"/>
@@ -1665,7 +1702,7 @@
         <v>576</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M35" t="str">
         <f t="shared" si="2"/>
@@ -1706,7 +1743,7 @@
         <v>584</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M37" t="str">
         <f t="shared" si="2"/>
@@ -1857,7 +1894,7 @@
         <v>832</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M43" t="str">
         <f t="shared" si="2"/>
@@ -1895,7 +1932,7 @@
         <v>896</v>
       </c>
       <c r="F45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M45" t="str">
         <f t="shared" si="2"/>
@@ -2229,7 +2266,7 @@
         <v>68</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I60" t="str">
         <f t="shared" si="1"/>
@@ -2304,7 +2341,7 @@
         <v>16</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I64" t="str">
         <f t="shared" si="1"/>
@@ -2428,10 +2465,10 @@
         <v>56</v>
       </c>
       <c r="F71" t="s">
+        <v>125</v>
+      </c>
+      <c r="G71" t="s">
         <v>53</v>
-      </c>
-      <c r="G71" t="s">
-        <v>54</v>
       </c>
       <c r="I71" t="str">
         <f t="shared" si="1"/>
@@ -2457,10 +2494,10 @@
         <v>64</v>
       </c>
       <c r="F72" t="s">
+        <v>54</v>
+      </c>
+      <c r="G72" t="s">
         <v>55</v>
-      </c>
-      <c r="G72" t="s">
-        <v>56</v>
       </c>
       <c r="I72" t="str">
         <f t="shared" si="1"/>
@@ -2491,7 +2528,7 @@
         <v>8</v>
       </c>
       <c r="F75" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="76" spans="2:13" x14ac:dyDescent="0.25">
@@ -2533,8 +2570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50946101-636E-4CAC-9348-8C1BCC50A424}">
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2574,7 +2611,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2">
         <v>72</v>
@@ -2664,7 +2701,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5">
         <v>96</v>
@@ -2724,7 +2761,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7">
         <v>112</v>
@@ -2740,7 +2777,7 @@
         <v>84</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="1"/>
@@ -2783,7 +2820,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9">
         <v>128</v>
@@ -2829,7 +2866,7 @@
         <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="1"/>
@@ -2902,7 +2939,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13">
         <v>160</v>
@@ -3232,7 +3269,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24">
         <v>264</v>
@@ -3262,7 +3299,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B25">
         <v>304</v>
@@ -3382,7 +3419,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B29">
         <v>344</v>
@@ -3412,7 +3449,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30">
         <v>352</v>
@@ -3442,7 +3479,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B31">
         <v>360</v>
@@ -3472,7 +3509,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B32">
         <v>368</v>
@@ -3562,7 +3599,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35">
         <v>440</v>
@@ -3592,7 +3629,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36">
         <v>448</v>
@@ -3652,7 +3689,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B38">
         <v>472</v>
@@ -3682,7 +3719,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B39">
         <v>480</v>
@@ -3699,7 +3736,7 @@
       </c>
       <c r="F39" t="str">
         <f t="shared" si="6"/>
-        <v>strings with floats</v>
+        <v>strings with floats, LocationFlag</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="7"/>
@@ -3712,7 +3749,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B40">
         <v>496</v>
@@ -3772,7 +3809,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B42">
         <v>536</v>
@@ -3802,13 +3839,13 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B43">
         <v>552</v>
       </c>
       <c r="F43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L43" t="str">
         <f t="shared" si="8"/>
@@ -3817,7 +3854,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B44">
         <v>560</v>
@@ -3847,7 +3884,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B45">
         <v>568</v>
@@ -3877,7 +3914,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B46">
         <v>576</v>
@@ -3907,7 +3944,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B47">
         <v>584</v>
@@ -3937,7 +3974,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B48">
         <v>592</v>
@@ -3967,7 +4004,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B49">
         <v>600</v>
@@ -3997,7 +4034,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B50">
         <v>656</v>
@@ -4027,7 +4064,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B51">
         <v>792</v>
@@ -4198,7 +4235,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B57">
         <v>904</v>
@@ -4228,7 +4265,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B58">
         <v>920</v>
@@ -4956,272 +4993,356 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74E2CD54-8002-4905-B0AC-525BD08EFB2E}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23:D24"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="2" width="78.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" t="s">
         <v>98</v>
-      </c>
-      <c r="B9" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" t="s">
         <v>100</v>
-      </c>
-      <c r="B10" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" t="s">
         <v>110</v>
-      </c>
-      <c r="C24" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B43" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43" t="s">
         <v>117</v>
-      </c>
-      <c r="C43" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C47" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D47" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C48" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>120</v>
+      </c>
+      <c r="B53" s="6">
+        <v>182883612</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>122</v>
+      </c>
+      <c r="B54" s="6">
+        <v>161535156</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>123</v>
+      </c>
+      <c r="B55" s="6">
+        <v>182452</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>121</v>
+      </c>
+      <c r="B56" s="6">
+        <f>B54-B55</f>
+        <v>161352704</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>124</v>
+      </c>
+      <c r="B57" s="6">
+        <f>B53-B56</f>
+        <v>21530908</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="6"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>126</v>
+      </c>
+      <c r="B60">
+        <v>50520856</v>
+      </c>
+      <c r="D60" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61" s="7"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>128</v>
+      </c>
+      <c r="B62">
+        <v>35152128</v>
+      </c>
+      <c r="C62">
+        <v>35966724</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>